<commit_message>
fix secDNSInterface for epp-16-dnssec-data-row-11
</commit_message>
<xml_diff>
--- a/data/epp-16-dnssec-data.xlsx
+++ b/data/epp-16-dnssec-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF68D67-B67E-814A-B1A5-8CCD6D1ACCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C1EE35-5EC0-CB48-A660-C28DE763BC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -333,16 +333,11 @@
   <dxfs count="14">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -368,11 +363,16 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -627,17 +627,17 @@
   </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{F151C1C9-FD61-3745-B6D9-436567D9F6F2}" name="action" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3D82AD55-769F-CD49-A19C-4CEE1C417D0E}" name="secDNSInterface" dataDxfId="0"/>
-    <tableColumn id="20" xr3:uid="{84610D9D-62D8-C747-BEB0-DA340D34D421}" name="keyTag" dataDxfId="10"/>
-    <tableColumn id="19" xr3:uid="{54D27880-56AD-DC42-BE78-EBB1A19D2339}" name="dsDataAlg" dataDxfId="9"/>
-    <tableColumn id="18" xr3:uid="{4C2A616C-31AB-9948-877D-701A0692DECD}" name="digestType" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{2467371F-CDC1-0443-9301-00252404EE8B}" name="digest" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{66E3B520-5E7B-914A-A7E7-5D2A0EC1B025}" name="flags" dataDxfId="6"/>
-    <tableColumn id="23" xr3:uid="{85CBAD45-FEDA-EF41-B68C-A469EEC82B26}" name="protocol" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{7BF4016C-657D-B647-BB2B-87573194BAB3}" name="keyDataAlg" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{D26FFFA2-9A10-9943-A61D-4B69D6D32E34}" name="pubKey" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3D82AD55-769F-CD49-A19C-4CEE1C417D0E}" name="secDNSInterface" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{84610D9D-62D8-C747-BEB0-DA340D34D421}" name="keyTag" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{54D27880-56AD-DC42-BE78-EBB1A19D2339}" name="dsDataAlg" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{4C2A616C-31AB-9948-877D-701A0692DECD}" name="digestType" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2467371F-CDC1-0443-9301-00252404EE8B}" name="digest" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{66E3B520-5E7B-914A-A7E7-5D2A0EC1B025}" name="flags" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{85CBAD45-FEDA-EF41-B68C-A469EEC82B26}" name="protocol" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{7BF4016C-657D-B647-BB2B-87573194BAB3}" name="keyDataAlg" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{D26FFFA2-9A10-9943-A61D-4B69D6D32E34}" name="pubKey" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -963,7 +963,7 @@
   <dimension ref="B2:AG39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1425,6 +1425,9 @@
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1441,9 +1444,6 @@
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>9</v>

</xml_diff>